<commit_message>
Cambios en el modo de ingestion de datos
</commit_message>
<xml_diff>
--- a/evidencia big data.xlsx
+++ b/evidencia big data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utmedu-my.sharepoint.com/personal/al03088785_tecmilenio_mx/Documents/TECMILENIO/Tareas 6to semestre/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utmedu-my.sharepoint.com/personal/al03088785_tecmilenio_mx/Documents/TECMILENIO/tareas 5to semestre/Repositorios/DataIngestion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="120" documentId="8_{3A01F0D1-F014-4140-9340-FC84EB091D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF8EB27C-7BF2-4925-85B3-43CF5340F21E}"/>
+  <xr:revisionPtr revIDLastSave="127" documentId="8_{3A01F0D1-F014-4140-9340-FC84EB091D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B7CD765-DA2B-4986-B9EC-3E845B6FB527}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B246943F-D56E-4C23-B4C6-713B909E6E01}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B246943F-D56E-4C23-B4C6-713B909E6E01}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -195,7 +195,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,7 +234,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -245,6 +249,29 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AFC9B4B2-1C20-455D-9E1E-AB6437FC6FC5}" name="Tabla1" displayName="Tabla1" ref="A2:N11" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A2:N11" xr:uid="{AFC9B4B2-1C20-455D-9E1E-AB6437FC6FC5}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{22AEB034-16F2-4793-9BCF-E650C86BA6BD}" name="Nombre tirador"/>
+    <tableColumn id="2" xr3:uid="{40066034-6F0A-4D92-AD15-4A17778F8437}" name="Edad"/>
+    <tableColumn id="3" xr3:uid="{B99AA3A3-590C-48F3-94D2-8E41502E40F3}" name="Experiencia"/>
+    <tableColumn id="4" xr3:uid="{CD74179E-C661-4407-9986-BA95D33F0095}" name="Distancia de tiro "/>
+    <tableColumn id="5" xr3:uid="{C11CFCB0-9BD5-48DA-8CDF-C2EE53D4C34C}" name="Angulo "/>
+    <tableColumn id="6" xr3:uid="{4F2C4352-0FF7-4AFD-80A7-C33A7DE7E2F4}" name="Altura de tirador"/>
+    <tableColumn id="7" xr3:uid="{6C6A138F-A73F-46C8-BE4A-B0C676077A6C}" name="Peso "/>
+    <tableColumn id="8" xr3:uid="{AA0AFC79-ADCA-4CC3-8309-46B60210029F}" name="Ambiente"/>
+    <tableColumn id="9" xr3:uid="{A7CE494F-00F3-4602-B36B-3A5E992D27CB}" name="Genero"/>
+    <tableColumn id="10" xr3:uid="{34EA8D6C-B0AE-427D-AB8F-7634AB22625E}" name="Peso del balon"/>
+    <tableColumn id="11" xr3:uid="{1CBA9CE9-0D9B-46AF-9405-FD425E78A80F}" name="Tiempo de tiro"/>
+    <tableColumn id="12" xr3:uid="{921D187B-4A4A-4817-A169-220944A1D1FC}" name="Tiro exitoso?"/>
+    <tableColumn id="13" xr3:uid="{12DBE661-9A0A-4D23-B747-9ED754FC5043}" name="Diestro / zurdo"/>
+    <tableColumn id="14" xr3:uid="{89995A09-25F8-45C0-9C33-5A896C054CE7}" name="Calibre de balon"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -567,21 +594,27 @@
   <dimension ref="A2:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -625,7 +658,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -669,7 +702,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -713,7 +746,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -757,7 +790,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -801,7 +834,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -845,7 +878,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -889,7 +922,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -933,7 +966,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -979,5 +1012,14 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{030e951d-6efd-42f5-8427-bab632cf8010}" enabled="0" method="" siteId="{030e951d-6efd-42f5-8427-bab632cf8010}" removed="1"/>
+</clbl:labelList>
 </file>
</xml_diff>